<commit_message>
modified bug get df rawdata
</commit_message>
<xml_diff>
--- a/DTProgram.xlsx
+++ b/DTProgram.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NickWork\tina-transform\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DC50B00-D09E-44A1-9DF8-6632E768B02D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BF67F30-612C-4E85-964C-B64DB7C422CD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2250" yWindow="2250" windowWidth="15375" windowHeight="7890" xr2:uid="{238E0772-73DA-46E7-A579-05C7B16F19D2}"/>
+    <workbookView xWindow="135" yWindow="480" windowWidth="12975" windowHeight="9165" xr2:uid="{238E0772-73DA-46E7-A579-05C7B16F19D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -71,9 +71,6 @@
     <t>F</t>
   </si>
   <si>
-    <t>C2</t>
-  </si>
-  <si>
     <t>≥</t>
   </si>
   <si>
@@ -117,6 +114,9 @@
   </si>
   <si>
     <t>Receive10%</t>
+  </si>
+  <si>
+    <t>C4</t>
   </si>
 </sst>
 </file>
@@ -153,8 +153,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -472,7 +473,7 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -512,10 +513,10 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C2" t="s">
         <v>10</v>
@@ -523,8 +524,8 @@
       <c r="D2">
         <v>20000</v>
       </c>
-      <c r="E2" t="s">
-        <v>11</v>
+      <c r="E2" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="F2" t="s">
         <v>11</v>
@@ -541,19 +542,19 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" t="s">
         <v>13</v>
-      </c>
-      <c r="B3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
       </c>
       <c r="D3">
         <v>3</v>
       </c>
-      <c r="E3" t="s">
-        <v>11</v>
+      <c r="E3" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="F3" t="s">
         <v>11</v>
@@ -570,16 +571,16 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s">
         <v>15</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4" t="s">
         <v>24</v>
-      </c>
-      <c r="C4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" t="s">
-        <v>25</v>
       </c>
       <c r="E4" t="s">
         <v>12</v>
@@ -591,55 +592,55 @@
         <v>11</v>
       </c>
       <c r="H4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modified hard logic C=>CT
</commit_message>
<xml_diff>
--- a/DTProgram.xlsx
+++ b/DTProgram.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Nick\Master Degree\Research\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NickWork\tina-transform\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE49F73F-DAA7-4A7A-9E2E-5050DDBAF6FB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E2B07EC-B971-4751-9D62-C5289EE461F8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3570" yWindow="1360" windowWidth="14400" windowHeight="7360" xr2:uid="{238E0772-73DA-46E7-A579-05C7B16F19D2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{238E0772-73DA-46E7-A579-05C7B16F19D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="33">
   <si>
     <t>ID</t>
   </si>
@@ -117,28 +118,72 @@
   </si>
   <si>
     <t>Receive10%</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>R?</t>
+  </si>
+  <si>
+    <t>C5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Tahoma"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="222"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="22"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="222"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -153,8 +198,29 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -471,17 +537,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F7AAC29-B523-440A-8A61-4E47F6B32AE9}">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="2.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.08203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -510,7 +576,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -539,7 +605,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -562,13 +628,13 @@
         <v>12</v>
       </c>
       <c r="H3" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="I3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -597,7 +663,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -611,7 +677,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -628,7 +694,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -645,4 +711,575 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A59E086-F28C-418F-BDDA-6556C2F4544D}">
+  <dimension ref="A1:S19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="13" width="10" style="1" customWidth="1"/>
+    <col min="14" max="14" width="11.28515625" style="1" customWidth="1"/>
+    <col min="15" max="18" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:19" ht="39" customHeight="1">
+      <c r="C1" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="2:19" ht="39" customHeight="1">
+      <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="2:19" ht="39" customHeight="1">
+      <c r="B3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="2:19" ht="39" customHeight="1">
+      <c r="B4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="2:19" ht="39" customHeight="1">
+      <c r="B5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="2:19" ht="39" customHeight="1"/>
+    <row r="7" spans="2:19" ht="39" customHeight="1">
+      <c r="B7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="2:19" ht="39" customHeight="1">
+      <c r="B8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="J8" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="K8" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="2:19" ht="39" customHeight="1">
+      <c r="B9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="2:19" ht="39" customHeight="1">
+      <c r="B10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="K10" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="2:19" ht="39" customHeight="1">
+      <c r="B11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="K11" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="2:19" ht="28.5">
+      <c r="B15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="2:19" ht="28.5">
+      <c r="B16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J16" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="K16" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="L16" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="M16" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="N16" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="O16" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="P16" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q16" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="R16" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="S16" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="2:19" ht="28.5">
+      <c r="B17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="J17" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="K17" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="L17" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="M17" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="N17" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="O17" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="P17" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q17" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="R17" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="S17" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="2:19" ht="28.5">
+      <c r="B18" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J18" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="K18" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="L18" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="M18" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="N18" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="O18" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="P18" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q18" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="R18" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="S18" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="2:19" ht="28.5">
+      <c r="B19" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="J19" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="K19" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="L19" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="M19" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="N19" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="O19" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="P19" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q19" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="R19" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="S19" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fixed bug muti dashs
</commit_message>
<xml_diff>
--- a/DTProgram.xlsx
+++ b/DTProgram.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NickWork\tina-transform\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71172FB3-17D6-426A-A5BF-AAB123A5D665}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3AF1525-C9BB-43AE-B5D4-53411761576A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{238E0772-73DA-46E7-A579-05C7B16F19D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1 (2)" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="29">
   <si>
     <t>ID</t>
   </si>
@@ -153,8 +154,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -469,10 +471,139 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F7AAC29-B523-440A-8A61-4E47F6B32AE9}">
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="2.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2">
+        <v>20000</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF885BA4-A6BC-4879-99A1-9C8BF005263C}">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -561,8 +692,8 @@
       <c r="G3" t="s">
         <v>12</v>
       </c>
-      <c r="H3" t="s">
-        <v>11</v>
+      <c r="H3" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="I3" t="s">
         <v>12</v>
@@ -634,6 +765,9 @@
       </c>
       <c r="B7" t="s">
         <v>28</v>
+      </c>
+      <c r="F7" t="s">
+        <v>18</v>
       </c>
       <c r="G7" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
fixed bug message json
</commit_message>
<xml_diff>
--- a/DTProgram.xlsx
+++ b/DTProgram.xlsx
@@ -1,20 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NickWork\tina-transform\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Nick\Master Degree\Research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{225437F1-9FC0-4D34-A031-F03C19831DC8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE49F73F-DAA7-4A7A-9E2E-5050DDBAF6FB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{238E0772-73DA-46E7-A579-05C7B16F19D2}"/>
+    <workbookView xWindow="3570" yWindow="1360" windowWidth="14400" windowHeight="7360" xr2:uid="{238E0772-73DA-46E7-A579-05C7B16F19D2}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1 (3)" sheetId="3" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="29">
   <si>
     <t>ID</t>
   </si>
@@ -64,6 +63,12 @@
   </si>
   <si>
     <t>&gt;</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>F</t>
   </si>
   <si>
     <t>C2</t>
@@ -118,11 +123,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Tahoma"/>
       <family val="2"/>
       <charset val="222"/>
       <scheme val="minor"/>
@@ -148,9 +153,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -166,55 +170,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>178082</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>256007</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>123167</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1106CEF3-BEB2-4E2B-9CF6-391093280F2A}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4200525" y="368582"/>
-          <a:ext cx="6323432" cy="3564585"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -513,20 +468,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67A22415-80A9-464B-858D-AE36727DBD2A}">
-  <dimension ref="A1:I4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F7AAC29-B523-440A-8A61-4E47F6B32AE9}">
+  <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.08203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -555,170 +510,139 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2">
+        <v>20000</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" t="s">
         <v>17</v>
       </c>
-      <c r="B2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" t="s">
-        <v>16</v>
+      <c r="I4" t="s">
+        <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
-      <c r="A3" t="s">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" t="s">
         <v>18</v>
       </c>
-      <c r="B3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I3" t="s">
-        <v>16</v>
+      <c r="G5" t="s">
+        <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
-      <c r="A4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" t="s">
-        <v>16</v>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" t="s">
+        <v>18</v>
+      </c>
+      <c r="I6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF885BA4-A6BC-4879-99A1-9C8BF005263C}">
-  <dimension ref="A1:E7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="2.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2">
-        <v>20000</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3">
-        <v>3</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>